<commit_message>
conclusão do arquivo pronto
</commit_message>
<xml_diff>
--- a/Guia 1 de Microcontroladores Tabelas e Mapas da 1 e 2 Questão.xlsx
+++ b/Guia 1 de Microcontroladores Tabelas e Mapas da 1 e 2 Questão.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ufma\5 periodo\arq. computadores\drive-download-20230324T153046Z-001\Guia1-20230614T182646Z-001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ufma\5 periodo\arq. computadores\P2_arquitetura de computadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1001,57 +1001,57 @@
     <xf numFmtId="0" fontId="12" fillId="13" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1746,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP940"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1772,30 +1772,30 @@
   <sheetData>
     <row r="1" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="54"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="49"/>
-      <c r="S1" s="50"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="44"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -1904,21 +1904,21 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="47"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="52" t="s">
+      <c r="S3" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="34"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="47"/>
       <c r="W3" s="4"/>
       <c r="X3" s="12"/>
       <c r="Y3" s="4"/>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="49" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="16" t="s">
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="4"/>
-      <c r="Q5" s="42" t="s">
+      <c r="Q5" s="52" t="s">
         <v>12</v>
       </c>
       <c r="R5" s="16" t="s">
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="36"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="16" t="s">
         <v>11</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="4"/>
-      <c r="Q6" s="36"/>
+      <c r="Q6" s="50"/>
       <c r="R6" s="16" t="s">
         <v>11</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="36"/>
+      <c r="J7" s="50"/>
       <c r="K7" s="16">
         <v>11</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="P7" s="4"/>
-      <c r="Q7" s="36"/>
+      <c r="Q7" s="50"/>
       <c r="R7" s="16">
         <v>11</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="37"/>
+      <c r="J8" s="51"/>
       <c r="K8" s="16">
         <v>10</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="4"/>
-      <c r="Q8" s="37"/>
+      <c r="Q8" s="51"/>
       <c r="R8" s="16">
         <v>10</v>
       </c>
@@ -2472,20 +2472,20 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="40"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="36"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="38" t="s">
+      <c r="S11" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="T11" s="39"/>
-      <c r="U11" s="40"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="36"/>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="12"/>
@@ -2706,11 +2706,11 @@
         <v>1</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="45"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -2826,12 +2826,12 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="32" t="s">
+      <c r="L17" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="34"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="47"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -2936,7 +2936,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="35" t="s">
+      <c r="J19" s="54" t="s">
         <v>12</v>
       </c>
       <c r="K19" s="16" t="s">
@@ -2992,7 +2992,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="36"/>
+      <c r="J20" s="50"/>
       <c r="K20" s="16" t="s">
         <v>11</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="36"/>
+      <c r="J21" s="50"/>
       <c r="K21" s="16">
         <v>11</v>
       </c>
@@ -3100,7 +3100,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="37"/>
+      <c r="J22" s="51"/>
       <c r="K22" s="16">
         <v>10</v>
       </c>
@@ -3200,11 +3200,11 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="38" t="s">
+      <c r="L24" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="39"/>
-      <c r="N24" s="40"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="36"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
@@ -3278,13 +3278,13 @@
     </row>
     <row r="26" spans="1:42" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -3483,16 +3483,16 @@
     </row>
     <row r="31" spans="1:42" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -3632,20 +3632,20 @@
       <c r="I34" s="31"/>
       <c r="J34" s="4"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="48" t="s">
+      <c r="L34" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="M34" s="49"/>
-      <c r="N34" s="50"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="44"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-      <c r="S34" s="48" t="s">
+      <c r="S34" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="T34" s="49"/>
-      <c r="U34" s="50"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="44"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
@@ -3728,21 +3728,21 @@
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
-      <c r="N36" s="51" t="s">
+      <c r="N36" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="34"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="46"/>
+      <c r="Q36" s="47"/>
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
-      <c r="U36" s="52" t="s">
+      <c r="U36" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="V36" s="33"/>
-      <c r="W36" s="33"/>
-      <c r="X36" s="34"/>
+      <c r="V36" s="46"/>
+      <c r="W36" s="46"/>
+      <c r="X36" s="47"/>
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
       <c r="AA36" s="4"/>
@@ -3848,7 +3848,7 @@
       <c r="I38" s="31"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="41" t="s">
+      <c r="L38" s="49" t="s">
         <v>12</v>
       </c>
       <c r="M38" s="16" t="s">
@@ -3867,7 +3867,7 @@
         <v>1</v>
       </c>
       <c r="R38" s="4"/>
-      <c r="S38" s="42" t="s">
+      <c r="S38" s="52" t="s">
         <v>12</v>
       </c>
       <c r="T38" s="16" t="s">
@@ -3923,7 +3923,7 @@
       <c r="I39" s="31"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="36"/>
+      <c r="L39" s="50"/>
       <c r="M39" s="16" t="s">
         <v>11</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="R39" s="4"/>
-      <c r="S39" s="36"/>
+      <c r="S39" s="50"/>
       <c r="T39" s="16" t="s">
         <v>11</v>
       </c>
@@ -3994,7 +3994,7 @@
       <c r="I40" s="31"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="36"/>
+      <c r="L40" s="50"/>
       <c r="M40" s="16">
         <v>11</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>1</v>
       </c>
       <c r="R40" s="4"/>
-      <c r="S40" s="36"/>
+      <c r="S40" s="50"/>
       <c r="T40" s="16">
         <v>11</v>
       </c>
@@ -4065,7 +4065,7 @@
       <c r="I41" s="31"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="37"/>
+      <c r="L41" s="51"/>
       <c r="M41" s="16">
         <v>10</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="R41" s="4"/>
-      <c r="S41" s="37"/>
+      <c r="S41" s="51"/>
       <c r="T41" s="16">
         <v>10</v>
       </c>
@@ -4240,20 +4240,20 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="38" t="s">
+      <c r="N44" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="O44" s="39"/>
-      <c r="P44" s="40"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="36"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
-      <c r="U44" s="38" t="s">
+      <c r="U44" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="V44" s="39"/>
-      <c r="W44" s="40"/>
+      <c r="V44" s="35"/>
+      <c r="W44" s="36"/>
       <c r="X44" s="4"/>
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
@@ -4449,11 +4449,11 @@
       <c r="I48" s="31"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="43" t="s">
+      <c r="L48" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M48" s="44"/>
-      <c r="N48" s="45"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="39"/>
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
@@ -4551,12 +4551,12 @@
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
-      <c r="N50" s="32" t="s">
+      <c r="N50" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="O50" s="33"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="34"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="46"/>
+      <c r="Q50" s="47"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
@@ -4657,7 +4657,7 @@
       <c r="I52" s="31"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="35" t="s">
+      <c r="L52" s="54" t="s">
         <v>12</v>
       </c>
       <c r="M52" s="16" t="s">
@@ -4718,7 +4718,7 @@
       <c r="I53" s="31"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
-      <c r="L53" s="36"/>
+      <c r="L53" s="50"/>
       <c r="M53" s="16" t="s">
         <v>11</v>
       </c>
@@ -4777,7 +4777,7 @@
       <c r="I54" s="31"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="36"/>
+      <c r="L54" s="50"/>
       <c r="M54" s="16">
         <v>11</v>
       </c>
@@ -4836,7 +4836,7 @@
       <c r="I55" s="31"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
-      <c r="L55" s="37"/>
+      <c r="L55" s="51"/>
       <c r="M55" s="16">
         <v>10</v>
       </c>
@@ -4946,11 +4946,11 @@
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
-      <c r="N57" s="38" t="s">
+      <c r="N57" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="O57" s="39"/>
-      <c r="P57" s="40"/>
+      <c r="O57" s="35"/>
+      <c r="P57" s="36"/>
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
       <c r="S57" s="4"/>
@@ -43558,6 +43558,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="N50:Q50"/>
+    <mergeCell ref="L52:L55"/>
+    <mergeCell ref="N57:P57"/>
+    <mergeCell ref="L38:L41"/>
+    <mergeCell ref="S38:S41"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="U44:W44"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="S34:U34"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="U36:X36"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="S11:U11"/>
     <mergeCell ref="J15:L15"/>
@@ -43572,19 +43585,6 @@
     <mergeCell ref="L17:O17"/>
     <mergeCell ref="J19:J22"/>
     <mergeCell ref="L24:N24"/>
-    <mergeCell ref="U44:W44"/>
-    <mergeCell ref="L48:N48"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="S34:U34"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="U36:X36"/>
-    <mergeCell ref="N50:Q50"/>
-    <mergeCell ref="L52:L55"/>
-    <mergeCell ref="N57:P57"/>
-    <mergeCell ref="L38:L41"/>
-    <mergeCell ref="S38:S41"/>
-    <mergeCell ref="N44:P44"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>